<commit_message>
Modificado Excel de prueba
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iván\git\Loader_e3b\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nombre</t>
   </si>
@@ -44,45 +44,6 @@
     <t>09940449X</t>
   </si>
   <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>C/ Real Oviedo 2</t>
-  </si>
-  <si>
-    <t>Av. De la Constitución 8</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
@@ -95,13 +56,37 @@
     <t>ana@example.com</t>
   </si>
   <si>
-    <t>Dirección postal</t>
+    <t>Juan Torres Pardo</t>
+  </si>
+  <si>
+    <t>Luis López Fernando</t>
+  </si>
+  <si>
+    <t>Ana Torres Pardo</t>
+  </si>
+  <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>32.21 45.34</t>
+  </si>
+  <si>
+    <t>76.14 98.54</t>
+  </si>
+  <si>
+    <t>76.34 57.73</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,11 +125,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -427,109 +410,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>